<commit_message>
Nueva migración desde Excel
</commit_message>
<xml_diff>
--- a/WebApp/Files/cargaDataBusccadorAndino.xlsx
+++ b/WebApp/Files/cargaDataBusccadorAndino.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arupo\Documents\dotNet\Buscador\WebApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB097E15-EB50-4594-AFC8-5E3495EAC497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D9E93C-5E9F-4F36-A943-2B523E321441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{227A6549-022C-499C-9D9D-BE9574C66532}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{227A6549-022C-499C-9D9D-BE9574C66532}"/>
   </bookViews>
   <sheets>
-    <sheet name="Esq1" sheetId="1" r:id="rId1"/>
-    <sheet name="esq2" sheetId="2" r:id="rId2"/>
+    <sheet name="GRILLA" sheetId="3" r:id="rId1"/>
+    <sheet name="ESQ_01" sheetId="2" r:id="rId2"/>
+    <sheet name="ESQ_02" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="39">
   <si>
     <t>sdfsf</t>
   </si>
@@ -140,14 +141,34 @@
   </si>
   <si>
     <t>brtbfgb</t>
+  </si>
+  <si>
+    <t>DataSistema</t>
+  </si>
+  <si>
+    <t>DataPais</t>
+  </si>
+  <si>
+    <t>SAE</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -175,10 +196,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,25 +514,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC73D135-DF39-4A2A-8C8C-E859C1F22551}">
-  <dimension ref="A1:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AE43D8-A90F-431E-8B7E-EF5425F0292A}">
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:O54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="7" width="20.5703125" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -526,29 +542,35 @@
       <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="F1">
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1">
         <v>41</v>
       </c>
-      <c r="G1">
+      <c r="I1">
         <v>42</v>
       </c>
-      <c r="H1">
+      <c r="J1">
         <v>43</v>
       </c>
-      <c r="I1">
+      <c r="K1">
         <v>44</v>
       </c>
-      <c r="J1">
+      <c r="L1">
         <v>45</v>
       </c>
-      <c r="K1">
+      <c r="M1">
         <v>46</v>
       </c>
-      <c r="L1">
+      <c r="N1">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -565,28 +587,34 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -594,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
         <v>45448</v>
@@ -603,28 +631,34 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -632,7 +666,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2">
         <v>45448</v>
@@ -641,28 +675,34 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>8</v>
       </c>
-      <c r="L4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -670,7 +710,7 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2">
         <v>45448</v>
@@ -679,28 +719,34 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2</v>
-      </c>
       <c r="J5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -708,7 +754,7 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <v>45448</v>
@@ -717,28 +763,34 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
         <v>6</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>9</v>
       </c>
-      <c r="L6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -746,7 +798,7 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2">
         <v>45448</v>
@@ -755,28 +807,34 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
       <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" t="s">
         <v>7</v>
       </c>
-      <c r="K7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -784,7 +842,7 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2">
         <v>45448</v>
@@ -793,28 +851,34 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
         <v>32</v>
       </c>
-      <c r="I8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>3</v>
-      </c>
       <c r="K8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
         <v>29</v>
       </c>
-      <c r="L8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -822,7 +886,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
         <v>45448</v>
@@ -831,28 +895,34 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
         <v>34</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
         <v>31</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -860,7 +930,7 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2">
         <v>45448</v>
@@ -869,28 +939,34 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>7</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>33</v>
       </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" t="s">
         <v>7</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>30</v>
       </c>
-      <c r="L10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -898,7 +974,7 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2">
         <v>45448</v>
@@ -907,28 +983,34 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
         <v>0</v>
       </c>
-      <c r="G11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
         <v>19</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>20</v>
       </c>
-      <c r="J11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" t="s">
         <v>21</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -936,7 +1018,7 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2">
         <v>45448</v>
@@ -945,28 +1027,34 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
         <v>6</v>
       </c>
-      <c r="H12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>2</v>
-      </c>
       <c r="J12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
         <v>6</v>
       </c>
-      <c r="K12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -974,7 +1062,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2">
         <v>45448</v>
@@ -983,28 +1071,34 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
         <v>6</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>9</v>
       </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" t="s">
         <v>6</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>9</v>
       </c>
-      <c r="L13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1012,7 +1106,7 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2">
         <v>45448</v>
@@ -1021,28 +1115,34 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
         <v>7</v>
       </c>
-      <c r="H14" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
       <c r="J14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" t="s">
         <v>7</v>
       </c>
-      <c r="K14" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1050,7 +1150,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2">
         <v>45448</v>
@@ -1059,28 +1159,34 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" t="s">
         <v>23</v>
       </c>
-      <c r="I15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>3</v>
-      </c>
       <c r="K15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" t="s">
         <v>26</v>
       </c>
-      <c r="L15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1088,7 +1194,7 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2">
         <v>45448</v>
@@ -1097,28 +1203,34 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
         <v>25</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" t="s">
         <v>28</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1126,7 +1238,7 @@
         <v>14</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2">
         <v>45448</v>
@@ -1135,28 +1247,34 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" t="s">
         <v>0</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>7</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>24</v>
       </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" t="s">
         <v>7</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>27</v>
       </c>
-      <c r="L17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1164,7 +1282,7 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2">
         <v>45448</v>
@@ -1173,43 +1291,1226 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>2</v>
-      </c>
       <c r="J18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" t="s">
         <v>6</v>
       </c>
-      <c r="K18" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7758C95F-DADF-4AED-9816-7F910A15EB1A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1">
+        <v>51</v>
+      </c>
+      <c r="I1">
+        <v>52</v>
+      </c>
+      <c r="J1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC73D135-DF39-4A2A-8C8C-E859C1F22551}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1">
+        <v>55</v>
+      </c>
+      <c r="I1">
+        <v>56</v>
+      </c>
+      <c r="J1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2">
+        <v>45448</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>